<commit_message>
Work on the updated plan for Home - Need to start in REVIT as well
</commit_message>
<xml_diff>
--- a/1_CAD/2024-03-24_BOQ.xlsx
+++ b/1_CAD/2024-03-24_BOQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AutoCAD\1_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468DBFCD-3AF3-4A7F-B28C-35436533BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E777E772-1DE0-4D9F-84B7-3A14B7CC6633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,8 +42,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="15015 - Personal View" guid="{CF7C4CCF-BD8F-4831-A134-79BE131FEC31}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="804" activeSheetId="1"/>
     <customWorkbookView name="QPUser - Personal View" guid="{1A456320-64A6-4F87-BF26-18A87C5BEF0F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="624" activeSheetId="3"/>
-    <customWorkbookView name="15015 - Personal View" guid="{CF7C4CCF-BD8F-4831-A134-79BE131FEC31}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="804" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
   <si>
     <t>Description</t>
   </si>
@@ -358,9 +358,6 @@
     <t>Lintels</t>
   </si>
   <si>
-    <t>Steel - Grade 80</t>
-  </si>
-  <si>
     <t>Gate</t>
   </si>
   <si>
@@ -439,13 +436,22 @@
     <t>Total COST:</t>
   </si>
   <si>
-    <t>Rough estimate from 5 marla ref.</t>
-  </si>
-  <si>
     <t>Assumed for Grade-80 from 60</t>
   </si>
   <si>
     <t>ft3</t>
+  </si>
+  <si>
+    <t>Reference from a 5 marla plot online costing ref.</t>
+  </si>
+  <si>
+    <t>Design (Drawings + Structural)</t>
+  </si>
+  <si>
+    <t>Steel - Grade 60</t>
+  </si>
+  <si>
+    <t>14 marlas x 2 (double storey)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -960,7 +966,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1003,10 +1009,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="16"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="16" applyFont="1"/>
-    <xf numFmtId="169" fontId="26" fillId="12" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="26" fillId="12" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="169" fontId="26" fillId="11" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="26" fillId="11" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="13" borderId="2" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1025,10 +1031,10 @@
     <xf numFmtId="0" fontId="21" fillId="14" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="27" fillId="12" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="12" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="27" fillId="11" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="11" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,33 +1058,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="2" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="3" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="4" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1096,9 +1075,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,6 +1165,39 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="19" fillId="9" borderId="1" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="19" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="2" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="3" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="4" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
@@ -1530,123 +1539,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
     </row>
     <row r="2" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
     </row>
     <row r="3" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
     </row>
     <row r="4" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
     </row>
     <row r="5" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
     </row>
     <row r="6" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
     </row>
     <row r="7" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="1:17" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -1664,36 +1673,36 @@
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="35" t="s">
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="41" t="s">
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="35" t="s">
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="76"/>
     </row>
     <row r="10" spans="1:17" ht="44.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="18" t="s">
         <v>31</v>
       </c>
@@ -1744,7 +1753,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="26">
         <v>45241</v>
       </c>
@@ -2344,46 +2353,46 @@
         <v>20</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="70" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B4" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="69" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" s="80" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B4" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="81" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="82">
-        <f>SUM('Main BOQ'!H12:H13,'Main BOQ'!H17)</f>
-        <v>7625000</v>
+      <c r="C5" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="72">
+        <f>SUM('Main BOQ'!H13:H14,'Main BOQ'!H18)</f>
+        <v>7925000</v>
       </c>
     </row>
     <row r="6" spans="2:4" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="82">
-        <f>SUM('Main BOQ'!H7:H11,'Main BOQ'!H14:H16,'Main BOQ'!H18:H20)</f>
+      <c r="C6" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="72">
+        <f>SUM('Main BOQ'!H8:H12,'Main BOQ'!H15:H17,'Main BOQ'!H19:H21)</f>
         <v>2554500</v>
       </c>
     </row>
@@ -2391,22 +2400,22 @@
       <c r="B7" s="10">
         <v>3</v>
       </c>
-      <c r="C7" s="81" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="82">
-        <f>SUM('Main BOQ'!H21:H23,'Main BOQ'!H6)</f>
-        <v>1820000</v>
+      <c r="C7" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="72">
+        <f>SUM('Main BOQ'!H22:H24,'Main BOQ'!H6)</f>
+        <v>3865000</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="12" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="83">
+        <v>123</v>
+      </c>
+      <c r="D8" s="73">
         <f>SUM(D5:D7)</f>
-        <v>11999500</v>
+        <v>14344500</v>
       </c>
     </row>
   </sheetData>
@@ -2421,550 +2430,578 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.88671875" style="44" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="46" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" style="46" customWidth="1"/>
-    <col min="6" max="7" width="15" style="46" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="46" customWidth="1"/>
-    <col min="9" max="9" width="33.88671875" style="47" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="44"/>
+    <col min="1" max="1" width="0.88671875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="37" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="37" customWidth="1"/>
+    <col min="6" max="7" width="15" style="37" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="37" customWidth="1"/>
+    <col min="9" max="9" width="44.88671875" style="38" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="35"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:9" ht="7.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" s="63" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B3" s="68" t="s">
+      <c r="C2" s="39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="53" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B3" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="66"/>
-    </row>
-    <row r="4" spans="2:9" s="49" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="C3" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-    </row>
-    <row r="5" spans="2:9" s="51" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="52" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+    </row>
+    <row r="4" spans="2:9" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+    </row>
+    <row r="5" spans="2:9" s="41" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="44" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="56">
+    <row r="6" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="46">
         <v>1</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="62"/>
+      <c r="E6" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="66">
+        <v>1</v>
+      </c>
+      <c r="G6" s="63">
+        <v>500000</v>
+      </c>
+      <c r="H6" s="64">
+        <f>F6*G6</f>
+        <v>500000</v>
+      </c>
+      <c r="I6" s="51"/>
+    </row>
+    <row r="7" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="46">
+        <f t="shared" ref="B7:B11" ca="1" si="0">OFFSET(B7,-1,0)+1</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="76">
+      <c r="D7" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="66">
         <v>1</v>
       </c>
-      <c r="G6" s="73">
+      <c r="G7" s="63">
         <f>75000</f>
         <v>75000</v>
       </c>
-      <c r="H6" s="74">
-        <f>F6*G6</f>
+      <c r="H7" s="64">
+        <f>F7*G7</f>
         <v>75000</v>
       </c>
-      <c r="I6" s="61" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="56">
-        <f t="shared" ref="B7:B10" ca="1" si="0">OFFSET(B7,-1,0)+1</f>
-        <v>2</v>
-      </c>
-      <c r="C7" s="71" t="s">
+      <c r="I7" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="46">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D8" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="76">
+      <c r="F8" s="66">
         <v>1</v>
       </c>
-      <c r="G7" s="73">
+      <c r="G8" s="63">
         <f>60000</f>
         <v>60000</v>
       </c>
-      <c r="H7" s="74">
-        <f t="shared" ref="H7:H23" si="1">F7*G7</f>
+      <c r="H8" s="64">
+        <f t="shared" ref="H8:H24" si="1">F8*G8</f>
         <v>60000</v>
       </c>
-      <c r="I7" s="61"/>
-    </row>
-    <row r="8" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="56">
+      <c r="I8" s="51"/>
+    </row>
+    <row r="9" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C8" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="76">
+      <c r="D9" s="62"/>
+      <c r="E9" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="66">
         <v>2400</v>
       </c>
-      <c r="G8" s="73">
+      <c r="G9" s="63">
         <v>90</v>
       </c>
-      <c r="H8" s="74">
+      <c r="H9" s="64">
         <f t="shared" si="1"/>
         <v>216000</v>
       </c>
-      <c r="I8" s="61"/>
-    </row>
-    <row r="9" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56">
+      <c r="I9" s="51"/>
+    </row>
+    <row r="10" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="76">
+      <c r="D10" s="62"/>
+      <c r="E10" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="66">
         <v>3600</v>
       </c>
-      <c r="G9" s="73">
+      <c r="G10" s="63">
         <v>135</v>
       </c>
-      <c r="H9" s="74">
+      <c r="H10" s="64">
         <f t="shared" si="1"/>
         <v>486000</v>
       </c>
-      <c r="I9" s="61"/>
-    </row>
-    <row r="10" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="56">
+      <c r="I10" s="51"/>
+    </row>
+    <row r="11" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="72"/>
-      <c r="E10" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="76">
+      <c r="D11" s="62"/>
+      <c r="E11" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="66">
         <v>7500</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G11" s="63">
         <v>40</v>
       </c>
-      <c r="H10" s="74">
+      <c r="H11" s="64">
         <f t="shared" si="1"/>
         <v>300000</v>
       </c>
-      <c r="I10" s="61"/>
-    </row>
-    <row r="11" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="56">
-        <f t="shared" ref="B11:B23" ca="1" si="2">OFFSET(B11,-1,0)+1</f>
-        <v>6</v>
-      </c>
-      <c r="C11" s="71" t="s">
+      <c r="I11" s="51"/>
+    </row>
+    <row r="12" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="46">
+        <f t="shared" ref="B12:B24" ca="1" si="2">OFFSET(B12,-1,0)+1</f>
+        <v>7</v>
+      </c>
+      <c r="C12" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="76">
+      <c r="D12" s="62"/>
+      <c r="E12" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="66">
         <v>3000</v>
       </c>
-      <c r="G11" s="73">
+      <c r="G12" s="63">
         <v>65</v>
       </c>
-      <c r="H11" s="74">
+      <c r="H12" s="64">
         <f t="shared" si="1"/>
         <v>195000</v>
       </c>
-      <c r="I11" s="61"/>
-    </row>
-    <row r="12" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="56">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="76">
-        <v>150000</v>
-      </c>
-      <c r="G12" s="73">
-        <v>16</v>
-      </c>
-      <c r="H12" s="74">
-        <f t="shared" si="1"/>
-        <v>2400000</v>
-      </c>
-      <c r="I12" s="61"/>
-    </row>
-    <row r="13" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="56">
+      <c r="I12" s="51"/>
+    </row>
+    <row r="13" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="46">
         <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
-      <c r="C13" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="76">
-        <v>1800</v>
-      </c>
-      <c r="G13" s="73">
-        <v>1250</v>
-      </c>
-      <c r="H13" s="74">
-        <f t="shared" ref="H13" si="3">F13*G13</f>
-        <v>2250000</v>
-      </c>
-      <c r="I13" s="61"/>
-    </row>
-    <row r="14" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="56">
+      <c r="C13" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="66">
+        <v>150000</v>
+      </c>
+      <c r="G13" s="63">
+        <v>18</v>
+      </c>
+      <c r="H13" s="64">
+        <f t="shared" si="1"/>
+        <v>2700000</v>
+      </c>
+      <c r="I13" s="51"/>
+    </row>
+    <row r="14" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="46">
         <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="66">
+        <v>1800</v>
+      </c>
+      <c r="G14" s="63">
+        <v>1250</v>
+      </c>
+      <c r="H14" s="64">
+        <f t="shared" ref="H14" si="3">F14*G14</f>
+        <v>2250000</v>
+      </c>
+      <c r="I14" s="51"/>
+    </row>
+    <row r="15" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="46">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="76">
+      <c r="D15" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="66">
         <v>1</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G15" s="63">
         <v>250000</v>
       </c>
-      <c r="H14" s="74">
+      <c r="H15" s="64">
         <f t="shared" si="1"/>
         <v>250000</v>
       </c>
-      <c r="I14" s="61"/>
-    </row>
-    <row r="15" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56">
+      <c r="I15" s="51"/>
+    </row>
+    <row r="16" spans="2:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="76">
+      <c r="D16" s="62"/>
+      <c r="E16" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="66">
         <v>1</v>
       </c>
-      <c r="G15" s="73">
+      <c r="G16" s="63">
         <v>25000</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H16" s="64">
         <f t="shared" si="1"/>
         <v>25000</v>
       </c>
-      <c r="I15" s="61"/>
-    </row>
-    <row r="16" spans="2:9" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="56">
+      <c r="I16" s="51"/>
+    </row>
+    <row r="17" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="76">
+      <c r="D17" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="66">
         <v>35</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G17" s="63">
         <v>8500</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H17" s="64">
         <f t="shared" si="1"/>
         <v>297500</v>
       </c>
-      <c r="I16" s="61"/>
-    </row>
-    <row r="17" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="56">
+      <c r="I17" s="51"/>
+    </row>
+    <row r="18" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="76">
+        <v>13</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="62"/>
+      <c r="E18" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="66">
         <v>8500</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G18" s="63">
         <v>350</v>
       </c>
-      <c r="H17" s="74">
+      <c r="H18" s="64">
         <f t="shared" si="1"/>
         <v>2975000</v>
       </c>
-      <c r="I17" s="61" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="56">
+      <c r="I18" s="51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="76">
+        <v>14</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="62"/>
+      <c r="E19" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="66">
         <v>1</v>
       </c>
-      <c r="G18" s="73">
+      <c r="G19" s="63">
         <v>250000</v>
       </c>
-      <c r="H18" s="74">
+      <c r="H19" s="64">
         <f t="shared" si="1"/>
         <v>250000</v>
       </c>
-      <c r="I18" s="61"/>
-    </row>
-    <row r="19" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="56">
+      <c r="I19" s="51"/>
+    </row>
+    <row r="20" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="76">
+        <v>15</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="66">
         <v>1</v>
       </c>
-      <c r="G19" s="73">
+      <c r="G20" s="63">
         <v>125000</v>
       </c>
-      <c r="H19" s="74">
+      <c r="H20" s="64">
         <f t="shared" si="1"/>
         <v>125000</v>
       </c>
-      <c r="I19" s="61"/>
-    </row>
-    <row r="20" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="56">
+      <c r="I20" s="51"/>
+    </row>
+    <row r="21" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="76">
+        <v>16</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="62"/>
+      <c r="E21" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="66">
         <v>1</v>
       </c>
-      <c r="G20" s="73">
+      <c r="G21" s="63">
         <v>350000</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H21" s="64">
         <f t="shared" si="1"/>
         <v>350000</v>
       </c>
-      <c r="I20" s="61"/>
-    </row>
-    <row r="21" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="56">
-        <f t="shared" ca="1" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="C21" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="76">
-        <v>3600</v>
-      </c>
-      <c r="G21" s="73">
-        <v>450</v>
-      </c>
-      <c r="H21" s="74">
-        <f t="shared" si="1"/>
-        <v>1620000</v>
-      </c>
-      <c r="I21" s="61"/>
-      <c r="J21" s="77"/>
-    </row>
-    <row r="22" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="56">
+      <c r="I21" s="51"/>
+    </row>
+    <row r="22" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="46">
         <f t="shared" ca="1" si="2"/>
         <v>17</v>
       </c>
-      <c r="C22" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="76">
+      <c r="C22" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="62"/>
+      <c r="E22" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="66">
+        <f>7200</f>
+        <v>7200</v>
+      </c>
+      <c r="G22" s="63">
+        <v>450</v>
+      </c>
+      <c r="H22" s="64">
+        <f t="shared" si="1"/>
+        <v>3240000</v>
+      </c>
+      <c r="I22" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="67"/>
+    </row>
+    <row r="23" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="46">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="62"/>
+      <c r="E23" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="66">
         <v>3</v>
       </c>
-      <c r="G22" s="73">
+      <c r="G23" s="63">
         <v>25000</v>
       </c>
-      <c r="H22" s="74">
+      <c r="H23" s="64">
         <f t="shared" si="1"/>
         <v>75000</v>
       </c>
-      <c r="I22" s="61"/>
-    </row>
-    <row r="23" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="56">
+      <c r="I23" s="51"/>
+    </row>
+    <row r="24" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="C23" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="76">
+        <v>19</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="62"/>
+      <c r="E24" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="66">
         <v>1</v>
       </c>
-      <c r="G23" s="73">
+      <c r="G24" s="63">
         <v>50000</v>
       </c>
-      <c r="H23" s="74">
+      <c r="H24" s="64">
         <f t="shared" si="1"/>
         <v>50000</v>
       </c>
-      <c r="I23" s="61"/>
-    </row>
-    <row r="24" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="70" t="s">
+      <c r="I24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="H24" s="75">
-        <f>SUM(H6:H23)</f>
-        <v>11999500</v>
-      </c>
-      <c r="I24" s="62"/>
+      <c r="H25" s="65">
+        <f>SUM(H6:H24)</f>
+        <v>14419500</v>
+      </c>
+      <c r="I25" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3002,12 +3039,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="2:5" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
@@ -3673,12 +3710,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4118,12 +4155,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4699,12 +4736,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">

</xml_diff>

<commit_message>
Extensive updated work and 3D views and walk through etc
</commit_message>
<xml_diff>
--- a/1_CAD/2024-03-24_BOQ.xlsx
+++ b/1_CAD/2024-03-24_BOQ.xlsx
@@ -8,42 +8,43 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AutoCAD\1_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E777E772-1DE0-4D9F-84B7-3A14B7CC6633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C21950-23A6-4C0C-8160-9AAC930921B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sched_tracking" sheetId="39" state="hidden" r:id="rId1"/>
     <sheet name="Summary" sheetId="27" r:id="rId2"/>
     <sheet name="Main BOQ" sheetId="26" r:id="rId3"/>
-    <sheet name="Phase-11" sheetId="40" state="hidden" r:id="rId4"/>
-    <sheet name="Phase-11b" sheetId="41" state="hidden" r:id="rId5"/>
-    <sheet name="Phase-13" sheetId="44" state="hidden" r:id="rId6"/>
-    <sheet name="Phase-14" sheetId="45" state="hidden" r:id="rId7"/>
+    <sheet name="Ref Videos" sheetId="46" r:id="rId4"/>
+    <sheet name="Phase-11" sheetId="40" state="hidden" r:id="rId5"/>
+    <sheet name="Phase-11b" sheetId="41" state="hidden" r:id="rId6"/>
+    <sheet name="Phase-13" sheetId="44" state="hidden" r:id="rId7"/>
+    <sheet name="Phase-14" sheetId="45" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_Fill" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="_Fill" localSheetId="3" hidden="1">#REF!</definedName>
     <definedName name="_Fill" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="_Fill" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Fill" localSheetId="6" hidden="1">#REF!</definedName>
+    <definedName name="_Fill" localSheetId="7" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Main BOQ'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Phase-11'!$B$3:$E$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Phase-11b'!$A$2:$D$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Phase-13'!$A$2:$D$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Phase-14'!$A$2:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Phase-11'!$B$3:$E$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Phase-11b'!$A$2:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Phase-13'!$A$2:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Phase-14'!$A$2:$D$25</definedName>
     <definedName name="wrn.OCS._.REPORT." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
-    <definedName name="wrn.OCS._.REPORT." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
     <definedName name="wrn.OCS._.REPORT." localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
     <definedName name="wrn.OCS._.REPORT." localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
     <definedName name="wrn.OCS._.REPORT." localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
+    <definedName name="wrn.OCS._.REPORT." localSheetId="7" hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
     <definedName name="wrn.OCS._.REPORT." hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="QPUser - Personal View" guid="{1A456320-64A6-4F87-BF26-18A87C5BEF0F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="624" activeSheetId="3"/>
     <customWorkbookView name="15015 - Personal View" guid="{CF7C4CCF-BD8F-4831-A134-79BE131FEC31}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="804" activeSheetId="1"/>
-    <customWorkbookView name="QPUser - Personal View" guid="{1A456320-64A6-4F87-BF26-18A87C5BEF0F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="624" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>Description</t>
   </si>
@@ -452,6 +453,18 @@
   </si>
   <si>
     <t>14 marlas x 2 (double storey)</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dy2pqZbFkRc</t>
+  </si>
+  <si>
+    <t>6.5 Crore 1 Kanal Entirely Different Designed House in DHA Lahore by CC Luxury</t>
+  </si>
+  <si>
+    <t>Video Description</t>
   </si>
 </sst>
 </file>
@@ -459,12 +472,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="52" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -771,6 +784,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -934,14 +971,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -961,12 +998,13 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1067,7 +1105,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="31" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1085,7 +1123,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="35" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
@@ -1103,10 +1141,10 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="36" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="39" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="41" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1121,7 +1159,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="42" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1133,7 +1171,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="44" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="44" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1154,7 +1192,7 @@
     <xf numFmtId="165" fontId="37" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="33" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1165,6 +1203,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="19" fillId="9" borderId="1" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="19" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="39" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="1" fontId="25" fillId="11" borderId="2" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1195,16 +1236,25 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="18" applyBorder="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{783CCA71-F4E3-43B5-9D10-A024D307E16C}"/>
     <cellStyle name="Comma 3" xfId="4" xr:uid="{AAB23110-F1D9-49A3-9F2B-8CD689E52B4D}"/>
     <cellStyle name="Comma 4" xfId="6" xr:uid="{F0F3DD3A-A334-4130-AB19-14DED889E60A}"/>
     <cellStyle name="Comma 4 2" xfId="14" xr:uid="{DA91D8AD-BD2E-447C-BC05-459EC09456EB}"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2 2" xfId="7" xr:uid="{0C1E1D1D-B9E5-4AD0-BBE7-B59687DB081E}"/>
@@ -1223,6 +1273,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFF6699"/>
       <color rgb="FFFF5050"/>
@@ -1539,123 +1590,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
     </row>
     <row r="2" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
     </row>
     <row r="3" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
     </row>
     <row r="4" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
     </row>
     <row r="5" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
     </row>
     <row r="6" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
     </row>
     <row r="7" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
     </row>
     <row r="8" spans="1:17" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -1673,36 +1724,36 @@
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="74" t="s">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="80" t="s">
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="74" t="s">
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="77"/>
     </row>
     <row r="10" spans="1:17" ht="44.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+      <c r="A10" s="80"/>
       <c r="B10" s="18" t="s">
         <v>31</v>
       </c>
@@ -1753,7 +1804,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="79"/>
+      <c r="A11" s="80"/>
       <c r="B11" s="26">
         <v>45241</v>
       </c>
@@ -2330,7 +2381,7 @@
   <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2432,8 +2483,8 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2473,16 +2524,16 @@
       <c r="I3" s="56"/>
     </row>
     <row r="4" spans="2:9" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
     </row>
     <row r="5" spans="2:9" s="41" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
@@ -2934,7 +2985,7 @@
         <f t="shared" si="1"/>
         <v>3240000</v>
       </c>
-      <c r="I22" s="84" t="s">
+      <c r="I22" s="74" t="s">
         <v>129</v>
       </c>
       <c r="J22" s="67"/>
@@ -3017,6 +3068,82 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E1FDFD-9569-4E6A-9430-8D7CCDAD7C09}">
+  <dimension ref="B3:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" style="85" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="85"/>
+    <col min="3" max="3" width="74.109375" style="85" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" style="85" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="85"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="90">
+        <v>1</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="90">
+        <v>2</v>
+      </c>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="90">
+        <v>3</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{61DCF24F-9761-416A-AE40-EEFF3C306DED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE36203-8160-49C9-9B40-E2620A070DBB}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
@@ -3039,12 +3166,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
     </row>
     <row r="3" spans="2:5" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
@@ -3689,7 +3816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428585E1-40D9-45AD-BDF5-27BAE1399CCB}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
@@ -3710,12 +3837,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4134,7 +4261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD27E8D2-BEFE-4EE4-9F09-2998275DAAFA}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
@@ -4155,12 +4282,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4715,7 +4842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E841D9D1-C746-401A-880A-1E017E42BEBE}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
@@ -4736,12 +4863,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">

</xml_diff>

<commit_message>
Excellent new 3D updates with new assets and REVIT import
</commit_message>
<xml_diff>
--- a/1_CAD/2024-03-24_BOQ.xlsx
+++ b/1_CAD/2024-03-24_BOQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AutoCAD\1_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C21950-23A6-4C0C-8160-9AAC930921B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADE0292-AA3C-42CF-B770-0D10CF75AA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,8 +43,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="15015 - Personal View" guid="{CF7C4CCF-BD8F-4831-A134-79BE131FEC31}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="804" activeSheetId="1"/>
     <customWorkbookView name="QPUser - Personal View" guid="{1A456320-64A6-4F87-BF26-18A87C5BEF0F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="624" activeSheetId="3"/>
-    <customWorkbookView name="15015 - Personal View" guid="{CF7C4CCF-BD8F-4831-A134-79BE131FEC31}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1276" windowHeight="804" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="136">
   <si>
     <t>Description</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>Video Description</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZX5UWi89m8M</t>
+  </si>
+  <si>
+    <t>17 Crore 1 Kanal Full Furnished ( COZY TRANQUILE ) Luxury House For Sale</t>
   </si>
 </sst>
 </file>
@@ -1206,36 +1212,6 @@
     <xf numFmtId="43" fontId="39" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="2" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="3" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="11" borderId="4" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1246,6 +1222,36 @@
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="2" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="3" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="11" borderId="4" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="25" fillId="10" borderId="1" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1590,123 +1596,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
     </row>
     <row r="2" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
     </row>
     <row r="3" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
     </row>
     <row r="4" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
     </row>
     <row r="5" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
     </row>
     <row r="7" spans="1:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
     </row>
     <row r="8" spans="1:17" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -1724,36 +1730,36 @@
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="75" t="s">
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="81" t="s">
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="75" t="s">
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="77"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="84"/>
     </row>
     <row r="10" spans="1:17" ht="44.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="80"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="18" t="s">
         <v>31</v>
       </c>
@@ -1804,7 +1810,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="26">
         <v>45241</v>
       </c>
@@ -2524,16 +2530,16 @@
       <c r="I3" s="56"/>
     </row>
     <row r="4" spans="2:9" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="90" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="2:9" s="41" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
@@ -3072,72 +3078,77 @@
   <dimension ref="B3:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" style="85" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="85"/>
-    <col min="3" max="3" width="74.109375" style="85" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" style="85" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="85"/>
+    <col min="1" max="1" width="5" style="75" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="75"/>
+    <col min="3" max="3" width="74.109375" style="75" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" style="75" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="75"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="77" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="90">
+      <c r="B4" s="80">
         <v>1</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="78" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="90">
+      <c r="B5" s="80">
         <v>2</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
+      <c r="C5" s="79" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="90">
+      <c r="B6" s="80">
         <v>3</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{61DCF24F-9761-416A-AE40-EEFF3C306DED}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{9973DC03-C279-4AE2-8525-1A1DE7A25AD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3166,12 +3177,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
     </row>
     <row r="3" spans="2:5" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
@@ -3837,12 +3848,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4282,12 +4293,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -4863,12 +4874,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">

</xml_diff>